<commit_message>
Fixed an error parsing step strings and color coded sequence generator.
</commit_message>
<xml_diff>
--- a/sequence_generator.xlsx
+++ b/sequence_generator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/kasper_arizona_edu/Documents/Research/Exponential Pump/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="279" documentId="8_{32553160-1EF7-4B28-8EA0-3BBFB24EDB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA035CAC-CE04-8342-89B2-BE8FA9DEAEE0}"/>
+  <xr:revisionPtr revIDLastSave="341" documentId="8_{32553160-1EF7-4B28-8EA0-3BBFB24EDB6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B5B7565C-603B-E343-8481-3D46C35C77BD}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20140" xr2:uid="{AA331077-8D97-4859-96A7-1B6D1DBCED24}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20080" xr2:uid="{AA331077-8D97-4859-96A7-1B6D1DBCED24}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Speed (RPM)</t>
   </si>
@@ -69,6 +69,12 @@
   </si>
   <si>
     <t>GROUPING</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>GROUP #</t>
   </si>
 </sst>
 </file>
@@ -99,15 +105,51 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFBFFB9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5FCFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -144,43 +186,146 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFA5FCFF"/>
+      <color rgb="FFFBFFB9"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -509,239 +654,423 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50EBF175-F5CC-4C53-A49E-A448CC5E178C}">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="7" width="30.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="7"/>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="17"/>
+      <c r="G1" s="24" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="19">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4">
         <v>30</v>
       </c>
-      <c r="B2">
+      <c r="C2" s="5">
         <v>2.7</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="29"/>
+      <c r="E2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11" t="str">
-        <f>_xlfn.CONCAT("&lt;",E2,",",E3,",",E4,"&gt;")</f>
+      <c r="G2" s="25" t="str">
+        <f>_xlfn.CONCAT("&lt;",F2,",",F3,",",F4,"&gt;")</f>
         <v>&lt;2.0,2.8,400&gt;</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>30</v>
-      </c>
-      <c r="B3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="19"/>
+      <c r="B3" s="4">
+        <v>40</v>
+      </c>
+      <c r="C3" s="5">
         <v>2.8</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="29"/>
+      <c r="E3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>30</v>
-      </c>
-      <c r="B4">
+      <c r="G3" s="26"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="19"/>
+      <c r="B4" s="4">
+        <v>50</v>
+      </c>
+      <c r="C4" s="5">
         <v>2.9</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="29"/>
+      <c r="E4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="22">
         <v>400</v>
       </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>30</v>
-      </c>
-      <c r="B5">
+      <c r="G4" s="27"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="19"/>
+      <c r="B5" s="4">
+        <v>64</v>
+      </c>
+      <c r="C5" s="5">
         <v>2.7</v>
       </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>30</v>
-      </c>
-      <c r="B6">
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="19"/>
+      <c r="B6" s="4">
+        <v>77</v>
+      </c>
+      <c r="C6" s="5">
         <v>2.8</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="18" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>30</v>
-      </c>
-      <c r="B7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="19">
+        <v>2</v>
+      </c>
+      <c r="B7" s="6">
+        <v>83</v>
+      </c>
+      <c r="C7" s="7">
         <v>2.9</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E8">
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="19"/>
+      <c r="B8" s="6">
+        <v>92</v>
+      </c>
+      <c r="C8" s="7">
+        <v>3.5</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="23">
         <v>1</v>
       </c>
-      <c r="F8" s="3" t="str">
-        <f>IF( NOT(COUNTA(A2:B6)), "",_xlfn.CONCAT("&lt;",_xlfn.TEXTJOIN(",","TRUE",A2:B6),"&gt;"))</f>
-        <v>&lt;30,2.7,30,2.8,30,2.9,30,2.7,30,2.8&gt;</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E9">
+      <c r="G8" s="4" t="str">
+        <f>IF( NOT(COUNTA(B2:C6)), "",_xlfn.CONCAT("&lt;",_xlfn.TEXTJOIN(",","TRUE",B2:C6),"&gt;"))</f>
+        <v>&lt;30,2.7,40,2.8,50,2.9,64,2.7,77,2.8&gt;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="19"/>
+      <c r="B9" s="6">
+        <v>104</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="23">
         <v>2</v>
       </c>
-      <c r="F9" s="3" t="str">
-        <f>IF( NOT(COUNTA(A7:B11)), "",_xlfn.CONCAT("&lt;",_xlfn.TEXTJOIN(",","TRUE",A7:B11),"&gt;"))</f>
-        <v>&lt;30,2.9&gt;</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="9"/>
-      <c r="E10">
+      <c r="G9" s="6" t="str">
+        <f>IF( NOT(COUNTA(B7:C11)), "",_xlfn.CONCAT("&lt;",_xlfn.TEXTJOIN(",","TRUE",B7:C11),"&gt;"))</f>
+        <v>&lt;83,2.9,92,3.5,104,4.0,112,5.6&gt;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="19"/>
+      <c r="B10" s="6">
+        <v>112</v>
+      </c>
+      <c r="C10" s="7">
+        <v>5.6</v>
+      </c>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="23">
         <v>3</v>
       </c>
-      <c r="F10" s="3" t="str">
-        <f>IF( NOT(COUNTA(A12:B16)), "",_xlfn.CONCAT("&lt;",_xlfn.TEXTJOIN(",","TRUE",A12:B16),"&gt;"))</f>
+      <c r="G10" s="8" t="str">
+        <f>IF( NOT(COUNTA(B12:C16)), "",_xlfn.CONCAT("&lt;",_xlfn.TEXTJOIN(",","TRUE",B12:C16),"&gt;"))</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="D11" s="9"/>
-      <c r="E11">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="19"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="23">
         <v>4</v>
       </c>
-      <c r="F11" s="3" t="str">
-        <f>IF( NOT(COUNTA(A17:B21)), "",_xlfn.CONCAT("&lt;",_xlfn.TEXTJOIN(",","TRUE",A17:B21),"&gt;"))</f>
+      <c r="G11" s="10" t="str">
+        <f>IF( NOT(COUNTA(B17:C21)), "",_xlfn.CONCAT("&lt;",_xlfn.TEXTJOIN(",","TRUE",B17:C21),"&gt;"))</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E12">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="19">
+        <v>3</v>
+      </c>
+      <c r="B12" s="8"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="23">
         <v>5</v>
       </c>
-      <c r="F12" s="3" t="str">
-        <f>IF( NOT(COUNTA(A22:B26)), "",_xlfn.CONCAT("&lt;",_xlfn.TEXTJOIN(",","TRUE",A22:B26),"&gt;"))</f>
+      <c r="G12" s="12" t="str">
+        <f>IF( NOT(COUNTA(B22:C26)), "",_xlfn.CONCAT("&lt;",_xlfn.TEXTJOIN(",","TRUE",B22:C26),"&gt;"))</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E13">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="19"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="23">
         <v>6</v>
       </c>
-      <c r="F13" s="3" t="str">
-        <f>IF( NOT(COUNTA(A27:B31)), "",_xlfn.CONCAT("&lt;",_xlfn.TEXTJOIN(",","TRUE",A27:B31),"&gt;"))</f>
+      <c r="G13" s="14" t="str">
+        <f>IF( NOT(COUNTA(B27:C31)), "",_xlfn.CONCAT("&lt;",_xlfn.TEXTJOIN(",","TRUE",B27:C31),"&gt;"))</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="3"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="3"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="3"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="3"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="3"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="F30" s="3"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="5"/>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="19"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="19"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="19"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="19">
+        <v>4</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="19"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="19"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" s="19"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" s="19"/>
+      <c r="B21" s="10"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" s="19">
+        <v>5</v>
+      </c>
+      <c r="B22" s="12"/>
+      <c r="C22" s="13"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="19"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="19"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="19"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="19"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="19">
+        <v>6</v>
+      </c>
+      <c r="B27" s="14"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="19"/>
+      <c r="B28" s="14"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" s="19"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" s="19"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" s="19"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="9">
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="F6:F7"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="C9" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>